<commit_message>
changed headlines in planning document to english from swedish. changed description in README file. fixed time plan to its correct version
</commit_message>
<xml_diff>
--- a/Project Time Plan.xlsx
+++ b/Project Time Plan.xlsx
@@ -61,9 +61,6 @@
     <t>ACTIVITY</t>
   </si>
   <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -178,10 +175,13 @@
     <t>Time Plan</t>
   </si>
   <si>
-    <t>Weekly work report</t>
-  </si>
-  <si>
-    <t>Write plan report</t>
+    <t>Write planning report</t>
+  </si>
+  <si>
+    <t>Oral Presentation</t>
+  </si>
+  <si>
+    <t>Halftime report</t>
   </si>
 </sst>
 </file>
@@ -908,7 +908,7 @@
   <dimension ref="B2:BQ34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -924,7 +924,7 @@
   <sheetData>
     <row r="2" spans="2:69" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -940,7 +940,7 @@
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="I3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -960,11 +960,11 @@
       </c>
       <c r="X3" s="12"/>
       <c r="Y3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AC3" s="13"/>
       <c r="AD3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
@@ -972,7 +972,7 @@
       <c r="AJ3" s="1"/>
       <c r="AK3" s="14"/>
       <c r="AL3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1234,7 +1234,7 @@
     </row>
     <row r="9" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -1254,7 +1254,7 @@
     </row>
     <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="16">
         <v>2</v>
@@ -1274,7 +1274,7 @@
     </row>
     <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="16">
         <v>2</v>
@@ -1294,7 +1294,7 @@
     </row>
     <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="16">
         <v>4</v>
@@ -1314,7 +1314,7 @@
     </row>
     <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="16">
         <v>1</v>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="16">
         <v>4</v>
@@ -1354,13 +1354,13 @@
     </row>
     <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="16">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D15" s="16">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E15" s="16">
         <v>0</v>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="16">
         <v>2</v>
@@ -1394,13 +1394,13 @@
     </row>
     <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="16">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" s="16">
         <v>0</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="18" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" s="16">
         <v>1</v>
@@ -1437,40 +1437,28 @@
         <v>25</v>
       </c>
       <c r="C19" s="18">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D19" s="16">
         <v>1</v>
       </c>
-      <c r="E19" s="16">
-        <v>0</v>
-      </c>
-      <c r="F19" s="16">
-        <v>0</v>
-      </c>
-      <c r="G19" s="17">
-        <v>0</v>
-      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
     </row>
     <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="16">
         <v>10</v>
       </c>
-      <c r="C20" s="16">
-        <v>9</v>
-      </c>
       <c r="D20" s="16">
-        <v>3</v>
-      </c>
-      <c r="E20" s="16">
-        <v>0</v>
-      </c>
-      <c r="F20" s="16">
-        <v>0</v>
-      </c>
-      <c r="G20" s="17">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
     </row>
     <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="15"/>

</xml_diff>

<commit_message>
before merge of documents
</commit_message>
<xml_diff>
--- a/Project Time Plan.xlsx
+++ b/Project Time Plan.xlsx
@@ -61,9 +61,6 @@
     <t>ACTIVITY</t>
   </si>
   <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -178,10 +175,13 @@
     <t>Time Plan</t>
   </si>
   <si>
-    <t>Weekly work report</t>
-  </si>
-  <si>
-    <t>Write plan report</t>
+    <t>Write planning report</t>
+  </si>
+  <si>
+    <t>Oral Presentation</t>
+  </si>
+  <si>
+    <t>Halftime report</t>
   </si>
 </sst>
 </file>
@@ -908,7 +908,7 @@
   <dimension ref="B2:BQ34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -924,7 +924,7 @@
   <sheetData>
     <row r="2" spans="2:69" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -940,7 +940,7 @@
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="I3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -960,11 +960,11 @@
       </c>
       <c r="X3" s="12"/>
       <c r="Y3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AC3" s="13"/>
       <c r="AD3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
@@ -972,7 +972,7 @@
       <c r="AJ3" s="1"/>
       <c r="AK3" s="14"/>
       <c r="AL3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1234,7 +1234,7 @@
     </row>
     <row r="9" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -1254,7 +1254,7 @@
     </row>
     <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="16">
         <v>2</v>
@@ -1274,7 +1274,7 @@
     </row>
     <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="16">
         <v>2</v>
@@ -1294,7 +1294,7 @@
     </row>
     <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="16">
         <v>4</v>
@@ -1314,7 +1314,7 @@
     </row>
     <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="16">
         <v>1</v>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="16">
         <v>4</v>
@@ -1354,13 +1354,13 @@
     </row>
     <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="16">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D15" s="16">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E15" s="16">
         <v>0</v>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="16">
         <v>2</v>
@@ -1394,13 +1394,13 @@
     </row>
     <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="16">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" s="16">
         <v>0</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="18" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" s="16">
         <v>1</v>
@@ -1437,40 +1437,28 @@
         <v>25</v>
       </c>
       <c r="C19" s="18">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D19" s="16">
         <v>1</v>
       </c>
-      <c r="E19" s="16">
-        <v>0</v>
-      </c>
-      <c r="F19" s="16">
-        <v>0</v>
-      </c>
-      <c r="G19" s="17">
-        <v>0</v>
-      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
     </row>
     <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="16">
         <v>10</v>
       </c>
-      <c r="C20" s="16">
-        <v>9</v>
-      </c>
       <c r="D20" s="16">
-        <v>3</v>
-      </c>
-      <c r="E20" s="16">
-        <v>0</v>
-      </c>
-      <c r="F20" s="16">
-        <v>0</v>
-      </c>
-      <c r="G20" s="17">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
     </row>
     <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="15"/>

</xml_diff>

<commit_message>
removed halftime report timeline from time plan document
</commit_message>
<xml_diff>
--- a/Project Time Plan.xlsx
+++ b/Project Time Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Plan</t>
   </si>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>Interviews and planning interviews</t>
-  </si>
-  <si>
-    <t>Write halftime report</t>
   </si>
   <si>
     <t>Write endreport</t>
@@ -460,7 +457,120 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -907,8 +1017,8 @@
   </sheetPr>
   <dimension ref="B2:BQ34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -924,7 +1034,7 @@
   <sheetData>
     <row r="2" spans="2:69" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -1337,10 +1447,10 @@
         <v>19</v>
       </c>
       <c r="C14" s="16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14" s="16">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E14" s="16">
         <v>0</v>
@@ -1357,10 +1467,10 @@
         <v>20</v>
       </c>
       <c r="C15" s="16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="16">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E15" s="16">
         <v>0</v>
@@ -1377,10 +1487,10 @@
         <v>21</v>
       </c>
       <c r="C16" s="16">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D16" s="16">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E16" s="16">
         <v>0</v>
@@ -1394,13 +1504,13 @@
     </row>
     <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" s="16">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D17" s="16">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E17" s="16">
         <v>0</v>
@@ -1416,28 +1526,22 @@
       <c r="B18" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="18">
+        <v>20</v>
+      </c>
+      <c r="D18" s="16">
         <v>1</v>
       </c>
-      <c r="D18" s="16">
-        <v>10</v>
-      </c>
-      <c r="E18" s="16">
-        <v>0</v>
-      </c>
-      <c r="F18" s="16">
-        <v>0</v>
-      </c>
-      <c r="G18" s="17">
-        <v>0</v>
-      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
     </row>
     <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="18">
-        <v>20</v>
+      <c r="C19" s="16">
+        <v>10</v>
       </c>
       <c r="D19" s="16">
         <v>1</v>
@@ -1447,15 +1551,9 @@
       <c r="G19" s="17"/>
     </row>
     <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="16">
-        <v>10</v>
-      </c>
-      <c r="D20" s="16">
-        <v>1</v>
-      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
       <c r="G20" s="17"/>
@@ -1577,38 +1675,38 @@
     <mergeCell ref="B2:G4"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:BP34">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="15" priority="4">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="14" priority="5">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="13" priority="6">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="12" priority="7">
       <formula>I$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:BP35">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:BP8">
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>I$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
lägger upp lite dokument
</commit_message>
<xml_diff>
--- a/Project Time Plan.xlsx
+++ b/Project Time Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="10515"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Plan</t>
   </si>
@@ -145,12 +145,6 @@
     <t xml:space="preserve"> Period Highlight:</t>
   </si>
   <si>
-    <t>Prestudy</t>
-  </si>
-  <si>
-    <t>Analyze LTE data</t>
-  </si>
-  <si>
     <t>Analyze available tools</t>
   </si>
   <si>
@@ -178,14 +172,59 @@
     <t>Oral Presentation</t>
   </si>
   <si>
-    <t>Halftime report</t>
+    <r>
+      <t>Prestudy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Analyze LTE data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>**</t>
+    </r>
+  </si>
+  <si>
+    <t>* We will study the air interface for LTE, i.e. How signals are sent between base station and user equipment, Scrum and interview techniques</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">** </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>We will study log files to better understand how we will build our lightweight analyzer</t>
+    </r>
+  </si>
+  <si>
+    <t>Halftime control</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -269,6 +308,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -382,7 +434,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -444,6 +496,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -457,120 +515,7 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -736,7 +681,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="10"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1017,8 +962,8 @@
   </sheetPr>
   <dimension ref="B2:BQ34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1034,7 +979,7 @@
   <sheetData>
     <row r="2" spans="2:69" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -1057,7 +1002,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
@@ -1343,8 +1288,8 @@
       <c r="BQ8" s="1"/>
     </row>
     <row r="9" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="15" t="s">
-        <v>14</v>
+      <c r="B9" s="21" t="s">
+        <v>23</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -1356,15 +1301,16 @@
         <v>1</v>
       </c>
       <c r="F9" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="17">
-        <v>0</v>
+        <f>(F9/D9)</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="15" t="s">
-        <v>15</v>
+      <c r="B10" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="C10" s="16">
         <v>2</v>
@@ -1379,18 +1325,19 @@
         <v>0</v>
       </c>
       <c r="G10" s="17">
+        <f t="shared" ref="G10:G19" si="0">(F10/D10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" s="16">
         <v>2</v>
       </c>
       <c r="D11" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="16">
         <v>0</v>
@@ -1399,12 +1346,13 @@
         <v>0</v>
       </c>
       <c r="G11" s="17">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" s="16">
         <v>4</v>
@@ -1419,12 +1367,13 @@
         <v>0</v>
       </c>
       <c r="G12" s="17">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" s="16">
         <v>1</v>
@@ -1433,18 +1382,19 @@
         <v>4</v>
       </c>
       <c r="E13" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="16">
         <v>0</v>
       </c>
       <c r="G13" s="17">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" s="16">
         <v>3</v>
@@ -1459,12 +1409,13 @@
         <v>0</v>
       </c>
       <c r="G14" s="17">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="16">
         <v>2</v>
@@ -1473,18 +1424,19 @@
         <v>10</v>
       </c>
       <c r="E15" s="16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="17">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="16">
         <v>16</v>
@@ -1499,12 +1451,13 @@
         <v>0</v>
       </c>
       <c r="G16" s="17">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" s="16">
         <v>1</v>
@@ -1519,12 +1472,13 @@
         <v>0</v>
       </c>
       <c r="G17" s="17">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="18">
         <v>20</v>
@@ -1532,13 +1486,20 @@
       <c r="D18" s="16">
         <v>1</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17"/>
+      <c r="E18" s="16">
+        <v>0</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0</v>
+      </c>
+      <c r="G18" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19" s="16">
         <v>10</v>
@@ -1546,9 +1507,16 @@
       <c r="D19" s="16">
         <v>1</v>
       </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
+      <c r="E19" s="16">
+        <v>0</v>
+      </c>
+      <c r="F19" s="16">
+        <v>0</v>
+      </c>
+      <c r="G19" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="15"/>
@@ -1575,7 +1543,9 @@
       <c r="G22" s="17"/>
     </row>
     <row r="23" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="15"/>
+      <c r="B23" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -1583,7 +1553,9 @@
       <c r="G23" s="17"/>
     </row>
     <row r="24" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="15"/>
+      <c r="B24" s="21" t="s">
+        <v>26</v>
+      </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -1591,7 +1563,6 @@
       <c r="G24" s="17"/>
     </row>
     <row r="25" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="15"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -1675,38 +1646,38 @@
     <mergeCell ref="B2:G4"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:BP34">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>I$8=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="3" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="2" priority="12">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35:BP35">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:BP8">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>I$8=period_selected</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>